<commit_message>
Do eq kill it?
</commit_message>
<xml_diff>
--- a/Report/Progress Bar.xlsx
+++ b/Report/Progress Bar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Samuel\workspace\METR4901\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA4963E1-D616-4D7C-A99A-907EEBEE0897}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F2375DC-BF84-458D-BA59-0910095F7618}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="27429" windowHeight="11023" xr2:uid="{EA1F1417-5E9D-4960-A68D-0B4549A49CFA}"/>
   </bookViews>
@@ -434,7 +434,7 @@
                   <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -717,7 +717,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>42</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -852,7 +852,7 @@
                   <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>61</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1249,7 +1249,7 @@
                   <c:v>11727</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>13112</c:v>
+                  <c:v>13659</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3532,8 +3532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{501ABB1B-0852-401E-B9D9-23AC9C720A04}">
   <dimension ref="A1:Y32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -3560,15 +3560,15 @@
       </c>
       <c r="C2">
         <f>SUM(B:B)</f>
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E2">
         <f>AVERAGE(E3:E23)</f>
-        <v>6</v>
+        <v>6.1428571428571432</v>
       </c>
       <c r="G2" s="5">
         <f>C2/C1</f>
-        <v>0.6</v>
+        <v>0.61428571428571432</v>
       </c>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
@@ -3879,21 +3879,21 @@
       </c>
       <c r="B13">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C13">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D13">
-        <v>13112</v>
+        <v>13659</v>
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F13">
         <f t="shared" si="4"/>
-        <v>1385</v>
+        <v>1932</v>
       </c>
       <c r="G13">
         <f t="shared" si="3"/>

</xml_diff>

<commit_message>
Vector of centrifugal and Coriolis forces
</commit_message>
<xml_diff>
--- a/Report/Progress Bar.xlsx
+++ b/Report/Progress Bar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Samuel\workspace\METR4901\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EF0E479-63A2-45AA-9737-ECF2ADA27C2C}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3970F3FB-F47E-4C28-B7FE-069984B7707C}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="27429" windowHeight="11023" xr2:uid="{EA1F1417-5E9D-4960-A68D-0B4549A49CFA}"/>
   </bookViews>
@@ -437,7 +437,7 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -720,7 +720,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>54</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -858,7 +858,7 @@
                   <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>73</c:v>
+                  <c:v>77</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1258,7 +1258,7 @@
                   <c:v>13787</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>14745</c:v>
+                  <c:v>15849</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3130,15 +3130,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>364671</xdr:colOff>
+      <xdr:colOff>197223</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>106135</xdr:rowOff>
+      <xdr:rowOff>111897</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>59871</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>590388</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>73478</xdr:rowOff>
+      <xdr:rowOff>79240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3204,15 +3204,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>446316</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>87086</xdr:rowOff>
+      <xdr:rowOff>174171</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>141516</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>391886</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>54429</xdr:rowOff>
+      <xdr:rowOff>141514</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3541,8 +3541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{501ABB1B-0852-401E-B9D9-23AC9C720A04}">
   <dimension ref="A1:Y32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -3569,15 +3569,15 @@
       </c>
       <c r="C2">
         <f>SUM(B:B)</f>
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="E2">
         <f>AVERAGE(E3:E23)</f>
-        <v>6.75</v>
+        <v>7.25</v>
       </c>
       <c r="G2" s="5">
         <f>C2/C1</f>
-        <v>0.36</v>
+        <v>0.38666666666666666</v>
       </c>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
@@ -3907,21 +3907,21 @@
       </c>
       <c r="B14">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C14">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D14">
-        <v>14745</v>
+        <v>15849</v>
       </c>
       <c r="E14">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="F14">
         <f t="shared" si="4"/>
-        <v>958</v>
+        <v>2062</v>
       </c>
       <c r="G14">
         <f t="shared" si="3"/>

</xml_diff>

<commit_message>
LM358AD - Low-Voltage Rail-to-Rail Output Operational Amplifier
</commit_message>
<xml_diff>
--- a/Report/Progress Bar.xlsx
+++ b/Report/Progress Bar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Samuel\workspace\METR4901\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79CF67A7-8F66-4FD9-AAEE-6A1F26B428E9}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{552B8C75-D686-40A0-A9F1-04F48F16BB8C}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="27429" windowHeight="11023" xr2:uid="{EA1F1417-5E9D-4960-A68D-0B4549A49CFA}"/>
   </bookViews>
@@ -1366,7 +1366,7 @@
                   <c:v>17862</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>19943</c:v>
+                  <c:v>20307</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3968,7 +3968,7 @@
   <dimension ref="A1:Y32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -4393,7 +4393,7 @@
         <v>106</v>
       </c>
       <c r="D16">
-        <v>19943</v>
+        <v>20307</v>
       </c>
       <c r="E16">
         <f t="shared" si="0"/>
@@ -4401,7 +4401,7 @@
       </c>
       <c r="F16">
         <f t="shared" si="4"/>
-        <v>2081</v>
+        <v>2445</v>
       </c>
       <c r="G16">
         <f t="shared" si="3"/>

</xml_diff>